<commit_message>
Deleting an extra column
</commit_message>
<xml_diff>
--- a/test_case_for_main_page.xlsx
+++ b/test_case_for_main_page.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="146">
   <si>
     <t xml:space="preserve">Идентификатор </t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Ожидаемый результат</t>
-  </si>
-  <si>
-    <t>Фактический результат</t>
   </si>
   <si>
     <t>Автор</t>
@@ -819,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -836,17 +833,16 @@
     <col min="7" max="7" width="56.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="57.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="69.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="45.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -861,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -869,762 +865,759 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G7" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="G10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G11" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="G14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="G15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G31" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="H32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G35" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G36" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H37" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H38" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="H39" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="I41" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G43" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="I45" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G46" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G47" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H49" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H50" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H51" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H52" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H53" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="I55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G56" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G57" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G58" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="I60" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G61" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G62" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="H63" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="H64" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="G66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="I66" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="G67" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G68" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>